<commit_message>
finalizei a parte de exportação/importação de dados
</commit_message>
<xml_diff>
--- a/ids_alunos_livros.xlsx
+++ b/ids_alunos_livros.xlsx
@@ -1,34 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Pojeto Biblioteca\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581CB3DE-B107-4182-8942-9DDF9C4D0531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ids_alunos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ids_livros" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ids_alunos" sheetId="1" r:id="rId1"/>
+    <sheet name="ids_livros" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TÍTULO</t>
+  </si>
+  <si>
+    <t>GÊNERO</t>
+  </si>
+  <si>
+    <t>AUTOR</t>
+  </si>
+  <si>
+    <t>EDITORA</t>
+  </si>
+  <si>
+    <t>QUANTIDADE</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>SERIE</t>
+  </si>
+  <si>
+    <t>TURNO</t>
+  </si>
+  <si>
+    <t>IDADE</t>
+  </si>
+  <si>
+    <t>CONTATO</t>
+  </si>
+  <si>
+    <t>ENDERECO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\(00\)\ 0\ 0000\-0000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,81 +95,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,137 +404,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1289</v>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Wellington</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>6391</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Rian</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>4005</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Pedro</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>9947</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Joaozinho</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>47</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>renner</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A pedra</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Eu</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criei o método de vinculação  identificadores únicos e atributos livros/alunos
</commit_message>
<xml_diff>
--- a/ids_alunos_livros.xlsx
+++ b/ids_alunos_livros.xlsx
@@ -1,83 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Pojeto Biblioteca\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581CB3DE-B107-4182-8942-9DDF9C4D0531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ids_alunos" sheetId="1" r:id="rId1"/>
-    <sheet name="ids_livros" sheetId="2" r:id="rId2"/>
+    <sheet name="ids_alunos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ids_livros" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>TÍTULO</t>
-  </si>
-  <si>
-    <t>GÊNERO</t>
-  </si>
-  <si>
-    <t>AUTOR</t>
-  </si>
-  <si>
-    <t>EDITORA</t>
-  </si>
-  <si>
-    <t>QUANTIDADE</t>
-  </si>
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>SERIE</t>
-  </si>
-  <si>
-    <t>TURNO</t>
-  </si>
-  <si>
-    <t>IDADE</t>
-  </si>
-  <si>
-    <t>CONTATO</t>
-  </si>
-  <si>
-    <t>ENDERECO</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\(00\)\ 0\ 0000\-0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,27 +49,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -404,87 +416,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25" style="1" customWidth="1"/>
+    <col width="17" customWidth="1" style="1" min="1" max="1"/>
+    <col width="18.28515625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="18.140625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="18.5703125" customWidth="1" style="1" min="4" max="5"/>
+    <col width="23.140625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="25" customWidth="1" style="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NOME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SERIE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>TURNO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IDADE</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>CONTATO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ENDERECO</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="1" customWidth="1"/>
+    <col width="18.28515625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="27.28515625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="26.28515625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="22.140625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="24.28515625" customWidth="1" style="1" min="5" max="5"/>
+    <col width="27.42578125" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TITULO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AUTOR</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EDITORA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>QUANTIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>TESTE1</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>gen1</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>aut 1</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>ed 1</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>TESTE2</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>gen2</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>aut 2</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>ed 2</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>